<commit_message>
renamed Id1008_check to Id10008_check
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
+++ b/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
@@ -6437,10 +6437,10 @@
     <t>2016 WHO Verbal Autopsy Form 1.5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">(Id1008_check) It is not possible to select that the respondent is the child of the deceased and enter that the deceased is a neonate or child. Please go back and correct the selection. </t>
-  </si>
-  <si>
-    <t>Id1008_check</t>
+    <t>Id10008_check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Id10008_check) It is not possible to select that the respondent is the child of the deceased and enter that the deceased is a neonate or child. Please go back and correct the selection. </t>
   </si>
 </sst>
 </file>
@@ -7323,8 +7323,8 @@
   <dimension ref="A1:M1020"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" customHeight="1"/>
@@ -8255,10 +8255,10 @@
         <v>619</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="C56" s="38" t="s">
         <v>2081</v>
-      </c>
-      <c r="C56" s="38" t="s">
-        <v>2080</v>
       </c>
       <c r="D56" s="38"/>
       <c r="E56" s="1" t="s">

</xml_diff>